<commit_message>
dropdown nama pekerjaan wbs
</commit_message>
<xml_diff>
--- a/data_wbs.xlsx
+++ b/data_wbs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Web Code</t>
   </si>
@@ -38,13 +38,22 @@
     <t>Uraian Kegiatan</t>
   </si>
   <si>
-    <t>2021-11-03</t>
-  </si>
-  <si>
-    <t>2021-11-04</t>
-  </si>
-  <si>
-    <t>2021-11-11</t>
+    <t>W0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VP </t>
+  </si>
+  <si>
+    <t>2021-11-12</t>
+  </si>
+  <si>
+    <t>2021-11-26</t>
+  </si>
+  <si>
+    <t>Instalasi jaringan</t>
+  </si>
+  <si>
+    <t>Membuat Instalasi jaringan</t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -415,67 +424,27 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>1212</v>
-      </c>
-      <c r="F2">
-        <v>1212</v>
-      </c>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>121</v>
-      </c>
-      <c r="F3">
-        <v>1212</v>
-      </c>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1212</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>221</v>
-      </c>
-      <c r="F4">
-        <v>112</v>
-      </c>
-      <c r="G4"/>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>